<commit_message>
Correct Miseq no run mode..
</commit_message>
<xml_diff>
--- a/docs/norseq.xlsx
+++ b/docs/norseq.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="40">
   <si>
     <t>HISEQ 2500:</t>
   </si>
@@ -607,7 +607,7 @@
   <dimension ref="A1:P31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -755,9 +755,6 @@
         <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
-      </c>
-      <c r="M6" t="s">
         <v>6</v>
       </c>
       <c r="P6" t="s">

</xml_diff>